<commit_message>
updated for longer runs and seed before initial values
</commit_message>
<xml_diff>
--- a/simulationStudy/simParamsSummary.xlsx
+++ b/simulationStudy/simParamsSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caitl\Documents\Postdoc\epidemicBCM\simulationStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFAD58F-A0E7-4EA1-B322-2920BFCE620A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7FC9C5-C9BC-44CA-BB85-A5127195DD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
+    <workbookView xWindow="5220" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,26 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="20">
-  <si>
-    <t>Threshold</t>
-  </si>
-  <si>
-    <t>Alarm</t>
-  </si>
-  <si>
-    <t>Delta</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="21">
   <si>
     <t>IType</t>
   </si>
   <si>
-    <t>Fixed</t>
-  </si>
-  <si>
-    <t>Dependence</t>
-  </si>
-  <si>
     <t>bw</t>
   </si>
   <si>
@@ -64,15 +49,9 @@
     <t>prev</t>
   </si>
   <si>
-    <t>Exp</t>
-  </si>
-  <si>
     <t>nu</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
@@ -91,10 +70,34 @@
     <t>Average</t>
   </si>
   <si>
-    <t>Hill</t>
-  </si>
-  <si>
-    <t>Power</t>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>x0</t>
+  </si>
+  <si>
+    <t>thresh</t>
+  </si>
+  <si>
+    <t>hill</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>alarmGen</t>
+  </si>
+  <si>
+    <t>smoothWindow</t>
+  </si>
+  <si>
+    <t>infPeriod</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -166,6 +169,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,66 +484,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564B3836-2B17-48DB-8114-869B4A6EAD37}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" style="3" customWidth="1"/>
     <col min="5" max="6" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="3"/>
-    <col min="11" max="11" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>14</v>
       </c>
       <c r="D2" s="4">
-        <v>14</v>
+        <v>0.36</v>
       </c>
       <c r="E2" s="4">
         <v>0.66</v>
@@ -549,23 +549,19 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="K2" s="4">
-        <f t="shared" ref="K2:K5" si="0">F2*1000000</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
+        <v>30</v>
       </c>
       <c r="D3" s="4">
-        <v>30</v>
+        <v>0.36</v>
       </c>
       <c r="E3" s="4">
         <v>0.66</v>
@@ -575,23 +571,19 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="K3" s="4">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.36</v>
       </c>
       <c r="E4" s="3">
         <v>0.68</v>
@@ -599,23 +591,19 @@
       <c r="F4" s="3">
         <v>1.2E-4</v>
       </c>
-      <c r="K4" s="8">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>0</v>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>30</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.36</v>
       </c>
       <c r="E5" s="3">
         <v>0.68</v>
@@ -623,23 +611,19 @@
       <c r="F5" s="3">
         <v>1E-4</v>
       </c>
-      <c r="K5" s="8">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.36</v>
       </c>
       <c r="E6" s="4">
         <v>0.7</v>
@@ -651,20 +635,19 @@
       <c r="H6" s="5">
         <v>140</v>
       </c>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="5">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.36</v>
       </c>
       <c r="E7" s="4">
         <v>0.7</v>
@@ -676,20 +659,19 @@
       <c r="H7" s="5">
         <v>80</v>
       </c>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>18</v>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.36</v>
       </c>
       <c r="E8" s="3">
         <v>0.68</v>
@@ -701,18 +683,18 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.36</v>
       </c>
       <c r="E9" s="3">
         <v>0.68</v>
@@ -724,18 +706,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.36</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -744,20 +726,19 @@
       <c r="I10" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="5">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.36</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -766,37 +747,36 @@
       <c r="I11" s="2">
         <v>1.8000000000000001E-4</v>
       </c>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>19</v>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>14</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.36</v>
       </c>
       <c r="I12" s="6">
         <v>3.5E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>19</v>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="C13" s="3">
+        <v>30</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.36</v>
       </c>
       <c r="I13" s="6">
         <v>2.0000000000000001E-4</v>
@@ -820,19 +800,19 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -840,10 +820,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>14</v>
@@ -879,10 +859,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -915,10 +895,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -954,10 +934,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>14</v>
@@ -990,10 +970,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -1026,10 +1006,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D7" s="7">
         <v>14</v>
@@ -1062,10 +1042,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D8" s="7">
         <v>30</v>
@@ -1098,10 +1078,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D9" s="7">
         <v>7</v>
@@ -1134,10 +1114,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D10" s="7">
         <v>14</v>
@@ -1170,10 +1150,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D11" s="7">
         <v>30</v>
@@ -1203,16 +1183,16 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1220,10 +1200,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -1241,10 +1221,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>30</v>
@@ -1259,10 +1239,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -1280,10 +1260,10 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>14</v>
@@ -1298,10 +1278,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>30</v>
@@ -1316,10 +1296,10 @@
         <v>6</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D20" s="7">
         <v>14</v>
@@ -1334,10 +1314,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D21" s="7">
         <v>30</v>
@@ -1352,10 +1332,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D22" s="7">
         <v>7</v>
@@ -1370,10 +1350,10 @@
         <v>9</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D23" s="7">
         <v>14</v>
@@ -1388,10 +1368,10 @@
         <v>10</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D24" s="7">
         <v>30</v>
@@ -1403,7 +1383,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -1411,10 +1391,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D27">
         <v>14</v>
@@ -1450,10 +1430,10 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D28">
         <v>30</v>
@@ -1489,10 +1469,10 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D29">
         <v>7</v>
@@ -1528,10 +1508,10 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D30">
         <v>14</v>
@@ -1567,10 +1547,10 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <v>30</v>
@@ -1606,10 +1586,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D32" s="7">
         <v>14</v>
@@ -1648,10 +1628,10 @@
         <v>7</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D33" s="7">
         <v>30</v>
@@ -1687,10 +1667,10 @@
         <v>8</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D34" s="7">
         <v>7</v>
@@ -1726,10 +1706,10 @@
         <v>9</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D35" s="7">
         <v>14</v>
@@ -1765,10 +1745,10 @@
         <v>10</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D36" s="7">
         <v>30</v>
@@ -1804,10 +1784,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D39">
         <v>14</v>
@@ -1818,10 +1798,10 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D40">
         <v>30</v>
@@ -1832,10 +1812,10 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -1846,10 +1826,10 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D42">
         <v>14</v>
@@ -1860,10 +1840,10 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D43">
         <v>30</v>
@@ -1874,10 +1854,10 @@
         <v>6</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D44" s="7">
         <v>14</v>
@@ -1888,10 +1868,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D45" s="7">
         <v>30</v>
@@ -1902,10 +1882,10 @@
         <v>8</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D46" s="7">
         <v>7</v>
@@ -1916,10 +1896,10 @@
         <v>9</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D47" s="7">
         <v>14</v>
@@ -1930,10 +1910,10 @@
         <v>10</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D48" s="7">
         <v>30</v>

</xml_diff>

<commit_message>
updated sim to include exponential infectious period:
</commit_message>
<xml_diff>
--- a/simulationStudy/simParamsSummary.xlsx
+++ b/simulationStudy/simParamsSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caitl\Documents\Postdoc\epidemicBCM\simulationStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7FC9C5-C9BC-44CA-BB85-A5127195DD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E140772-ABCB-4933-9E2A-4C194E8F5385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="22">
   <si>
     <t>IType</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>infPeriod</t>
+  </si>
+  <si>
+    <t>rateI</t>
   </si>
 </sst>
 </file>
@@ -484,22 +487,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564B3836-2B17-48DB-8114-869B4A6EAD37}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="3"/>
+    <col min="4" max="5" width="9.5546875" style="3" customWidth="1"/>
+    <col min="6" max="7" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -513,22 +516,25 @@
         <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -541,16 +547,17 @@
       <c r="D2" s="4">
         <v>0.36</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4">
         <v>0.66</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>1E-4</v>
       </c>
-      <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -563,16 +570,17 @@
       <c r="D3" s="4">
         <v>0.36</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4">
         <v>0.66</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
@@ -583,16 +591,19 @@
         <v>14</v>
       </c>
       <c r="D4" s="8">
-        <v>0.36</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.68</v>
+        <v>0.42</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.1429</v>
       </c>
       <c r="F4" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G4" s="3">
         <v>1.2E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
@@ -603,16 +614,19 @@
         <v>30</v>
       </c>
       <c r="D5" s="8">
-        <v>0.36</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.68</v>
+        <v>0.42</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.1429</v>
       </c>
       <c r="F5" s="3">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0.78</v>
+      </c>
+      <c r="G5" s="3">
+        <v>6.9999999999999994E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -625,18 +639,19 @@
       <c r="D6" s="4">
         <v>0.36</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
         <v>0.7</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5">
         <v>5</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -649,18 +664,19 @@
       <c r="D7" s="4">
         <v>0.36</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
         <v>0.7</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
         <v>5</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -671,19 +687,22 @@
         <v>14</v>
       </c>
       <c r="D8" s="8">
-        <v>0.36</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.68</v>
-      </c>
-      <c r="G8" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.1429</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H8" s="3">
         <v>5</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -694,19 +713,22 @@
         <v>30</v>
       </c>
       <c r="D9" s="8">
-        <v>0.36</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.68</v>
-      </c>
-      <c r="G9" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.1429</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="H9" s="3">
         <v>5</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -719,15 +741,16 @@
       <c r="D10" s="4">
         <v>0.36</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="2">
+      <c r="I10" s="5"/>
+      <c r="J10" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -740,15 +763,16 @@
       <c r="D11" s="4">
         <v>0.36</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="2">
+      <c r="I11" s="5"/>
+      <c r="J11" s="2">
         <v>1.8000000000000001E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -759,13 +783,16 @@
         <v>14</v>
       </c>
       <c r="D12" s="8">
-        <v>0.36</v>
-      </c>
-      <c r="I12" s="6">
-        <v>3.5E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.42</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.1429</v>
+      </c>
+      <c r="J12" s="6">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
@@ -776,10 +803,13 @@
         <v>30</v>
       </c>
       <c r="D13" s="8">
-        <v>0.36</v>
-      </c>
-      <c r="I13" s="6">
-        <v>2.0000000000000001E-4</v>
+        <v>0.42</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.1429</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1.8000000000000001E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>